<commit_message>
Model execution, rewind and replay changes and fixes
</commit_message>
<xml_diff>
--- a/model/processed_output00N0-JSEE.xlsx
+++ b/model/processed_output00N0-JSEE.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t xml:space="preserve">ExecutionDate</t>
   </si>
@@ -141,7 +141,7 @@
     <t>00N0-JSEE</t>
   </si>
   <si>
-    <t>0.0</t>
+    <t>35.78</t>
   </si>
   <si>
     <t>202410</t>
@@ -153,6 +153,9 @@
     <t>LEGAL PRINCIPAL</t>
   </si>
   <si>
+    <t>-11.64</t>
+  </si>
+  <si>
     <t>2024-10-28</t>
   </si>
   <si>
@@ -162,7 +165,7 @@
     <t>SPORTING GOODS AND OUTDOORS</t>
   </si>
   <si>
-    <t>Mon Oct 28 00:30:00 IST 2024</t>
+    <t>Mon Oct 28 00:00:00 IST 2024</t>
   </si>
   <si>
     <t>2024-11-28</t>
@@ -748,54 +751,54 @@
     </row>
     <row r="2">
       <c r="B2" t="s" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
       </c>
       <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
-      </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -865,7 +868,7 @@
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
         <v>40</v>

</xml_diff>